<commit_message>
terminata BOM di acquisti
</commit_message>
<xml_diff>
--- a/hw-panelization/50-000-Produzione CS-SB000/acquisti_BOM.xlsx
+++ b/hw-panelization/50-000-Produzione CS-SB000/acquisti_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="124">
   <si>
     <t>Id</t>
   </si>
@@ -298,6 +298,99 @@
   </si>
   <si>
     <t>http://www.mouser.it/ProductDetail/Panasonic-Industrial-Devices/AQZ204/?qs=sGAEpiMZZMsUriz2CNI3E9Evjuv1TJ6f2a2N4%2f3G9wQ%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/Vishay-Vitramon/VJ0603Y104KXXCW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQNbg85K4ab%2f3y6VBJhgKFs4%3d</t>
+  </si>
+  <si>
+    <t>VJ0603Y104KXXCW1BC</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/Taiyo-Yuden/TMK107B7105KA-T/?qs=sGAEpiMZZMs0AnBnWHyRQAEIN6r3SS%2fOl79Ozz7Y7A0%3d</t>
+  </si>
+  <si>
+    <t>TMK107B7105KA-T</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/Vishay-Vitramon/VJ0603Y103KXACW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQNbg85K4ab%2f3XqRx2jQHGsc%3d</t>
+  </si>
+  <si>
+    <t>VJ0603Y103KXACW1BC</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/FCI/76341-304LF/?qs=sGAEpiMZZMvffgRu4KC1R04q9MI2j2SgEoX0VzuNj44%3d</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>76341-304LF</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/Search/ProductDetail.aspx?qs=5xI8GKdkXll%2f8E%252bQi8rpbg%3d%3d</t>
+  </si>
+  <si>
+    <t>DBG</t>
+  </si>
+  <si>
+    <t>77311-101-04LF</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/OSRAM-Opto-Semiconductors/LB-Q39G-L2N2-35-1/?qs=sGAEpiMZZMtilyJihmhKqw6XzfZqY0e%2f0qyczb4i18U%3d</t>
+  </si>
+  <si>
+    <t>OSRAM</t>
+  </si>
+  <si>
+    <t>LB Q39G-L2N2-35-1</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/AVX/TAJA475K025RNJ/?qs=sGAEpiMZZMuEN2agSAc2psTMe46DsJuTkp2PmPWavjw%3d</t>
+  </si>
+  <si>
+    <t>TAJA475K025RNJ</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/TDK/MPZ1608S601ATD25/?qs=sGAEpiMZZMukHu%252bjC5l7YbCeHRK7sEncw0fmqz%2fRw6Y%3d</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MPZ1608S601ATD25</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/AVX/SMAJ220CA/?qs=sGAEpiMZZMuNo3spt1BaV66PehheyE98%252bzR6pJjYVkI%3d</t>
+  </si>
+  <si>
+    <t>SMAJ220CA</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/TE-Connectivity/282834-4/?qs=sGAEpiMZZMvZTcaMAxB2AJ%2f79sE4hFAYjYMQvvFyg9w%3d</t>
+  </si>
+  <si>
+    <t>282834-4</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/TE-Connectivity/282834-2/?qs=sGAEpiMZZMvZTcaMAxB2AJ%2f79sE4hFAYo1Yb6cyIxXA%3d</t>
+  </si>
+  <si>
+    <t>282834-2</t>
+  </si>
+  <si>
+    <t>http://www.mouser.it/ProductDetail/TE-Connectivity/2013499-1/?qs=%2fha2pyFaduhRZht4SACbfCn5uv%2fFK7O4gTjERbAiA5DS8vYJFtEZW0iQLVW1GcC7</t>
+  </si>
+  <si>
+    <t>2013499-1</t>
   </si>
 </sst>
 </file>
@@ -654,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +914,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M5" si="1">K4*L4</f>
+        <f t="shared" ref="M4:M7" si="1">K4*L4</f>
         <v>0.8</v>
       </c>
     </row>
@@ -883,11 +976,30 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="H6" t="s">
         <v>61</v>
       </c>
       <c r="I6" t="s">
         <v>57</v>
+      </c>
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>5.28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -906,11 +1018,30 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="H7" t="s">
         <v>62</v>
       </c>
       <c r="I7" t="s">
         <v>57</v>
+      </c>
+      <c r="J7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24" x14ac:dyDescent="0.25">
@@ -951,7 +1082,7 @@
         <v>0.112</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M10" si="2">K8*L8</f>
+        <f t="shared" ref="M8:M12" si="2">K8*L8</f>
         <v>11.200000000000001</v>
       </c>
     </row>
@@ -1055,11 +1186,30 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
       <c r="H11" t="s">
         <v>60</v>
       </c>
       <c r="I11" t="s">
         <v>57</v>
+      </c>
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>2.3E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1078,12 +1228,31 @@
       <c r="E12" t="s">
         <v>29</v>
       </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H12" t="s">
         <v>60</v>
       </c>
       <c r="I12" t="s">
         <v>57</v>
       </c>
+      <c r="J12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0.36</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1123,7 +1292,7 @@
         <v>0.94699999999999995</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M16" si="3">K13*L13</f>
+        <f t="shared" ref="M13:M17" si="3">K13*L13</f>
         <v>9.4699999999999989</v>
       </c>
     </row>
@@ -1269,11 +1438,30 @@
       <c r="E17" t="s">
         <v>15</v>
       </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="H17" t="s">
         <v>61</v>
       </c>
       <c r="I17" t="s">
         <v>58</v>
+      </c>
+      <c r="J17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>5.28</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1292,11 +1480,26 @@
       <c r="E18" t="s">
         <v>18</v>
       </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="H18" t="s">
         <v>62</v>
       </c>
       <c r="I18" t="s">
         <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1337,7 +1540,7 @@
         <v>10.8</v>
       </c>
       <c r="M19">
-        <f t="shared" ref="M19" si="4">K19*L19</f>
+        <f t="shared" ref="M19:M21" si="4">K19*L19</f>
         <v>10.8</v>
       </c>
     </row>
@@ -1357,11 +1560,30 @@
       <c r="E20" t="s">
         <v>27</v>
       </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
       <c r="H20" t="s">
         <v>60</v>
       </c>
       <c r="I20" t="s">
         <v>58</v>
+      </c>
+      <c r="J20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <v>2.3E-2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1380,12 +1602,31 @@
       <c r="E21" t="s">
         <v>29</v>
       </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H21" t="s">
         <v>60</v>
       </c>
       <c r="I21" t="s">
         <v>58</v>
       </c>
+      <c r="J21" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1425,7 +1666,7 @@
         <v>4.26</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22" si="5">K22*L22</f>
+        <f t="shared" ref="M22:M23" si="5">K22*L22</f>
         <v>4.26</v>
       </c>
     </row>
@@ -1445,11 +1686,30 @@
       <c r="E23" t="s">
         <v>37</v>
       </c>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="H23" t="s">
         <v>61</v>
       </c>
       <c r="I23" t="s">
         <v>59</v>
+      </c>
+      <c r="J23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="5"/>
+        <v>5.28</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1468,11 +1728,30 @@
       <c r="E24" t="s">
         <v>27</v>
       </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
       <c r="H24" t="s">
         <v>60</v>
       </c>
       <c r="I24" t="s">
         <v>59</v>
+      </c>
+      <c r="J24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>2.3E-2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M29" si="6">K24*L24</f>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1491,11 +1770,30 @@
       <c r="E25" t="s">
         <v>29</v>
       </c>
+      <c r="F25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H25" t="s">
         <v>60</v>
       </c>
       <c r="I25" t="s">
         <v>59</v>
+      </c>
+      <c r="J25" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="6"/>
+        <v>0.36</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1514,11 +1812,30 @@
       <c r="E26" t="s">
         <v>41</v>
       </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="H26" t="s">
         <v>60</v>
       </c>
       <c r="I26" t="s">
         <v>59</v>
+      </c>
+      <c r="J26" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1.01</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="6"/>
+        <v>1.01</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1537,11 +1854,30 @@
       <c r="E27" t="s">
         <v>43</v>
       </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>99</v>
+      </c>
       <c r="H27" t="s">
         <v>60</v>
       </c>
       <c r="I27" t="s">
         <v>59</v>
+      </c>
+      <c r="J27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27">
+        <v>50</v>
+      </c>
+      <c r="L27">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="6"/>
+        <v>2.25</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1560,11 +1896,30 @@
       <c r="E28" t="s">
         <v>46</v>
       </c>
+      <c r="F28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="H28" t="s">
         <v>63</v>
       </c>
       <c r="I28" t="s">
         <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28">
+        <v>20</v>
+      </c>
+      <c r="L28">
+        <v>0.125</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="6"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1583,11 +1938,30 @@
       <c r="E29" t="s">
         <v>49</v>
       </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" t="s">
+        <v>114</v>
+      </c>
       <c r="H29" t="s">
         <v>66</v>
       </c>
       <c r="I29" t="s">
         <v>59</v>
+      </c>
+      <c r="J29" t="s">
+        <v>112</v>
+      </c>
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="6"/>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1628,7 +2002,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M31" si="6">K30*L30</f>
+        <f t="shared" ref="M30:M32" si="7">K30*L30</f>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -1670,7 +2044,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="M31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -1690,22 +2064,123 @@
       <c r="E32" t="s">
         <v>55</v>
       </c>
+      <c r="F32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="H32" t="s">
         <v>61</v>
       </c>
       <c r="I32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>122</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1.61</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="7"/>
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
       <c r="M33">
         <f>SUM(M2:M32)</f>
-        <v>56.109999999999992</v>
+        <v>85.155000000000015</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" t="s">
+        <v>61</v>
+      </c>
+      <c r="I35" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" t="s">
+        <v>103</v>
+      </c>
+      <c r="K35">
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ref="M35:M36" si="8">K35*L35</f>
+        <v>1.9900000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H36" t="s">
+        <v>61</v>
+      </c>
+      <c r="I36" t="s">
+        <v>104</v>
+      </c>
+      <c r="J36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="M36">
+        <f>K36*L36</f>
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" t="s">
+        <v>104</v>
+      </c>
+      <c r="J37" t="s">
+        <v>120</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="M37">
+        <f>K37*L37</f>
+        <v>0.78700000000000003</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>